<commit_message>
delete an organization without teams and being an administrator
</commit_message>
<xml_diff>
--- a/Tasks/Views.xlsx
+++ b/Tasks/Views.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>MockUp</t>
   </si>
@@ -121,7 +121,7 @@
     <t>Eliminar organization (grupo) si no tiene equipos</t>
   </si>
   <si>
-    <t>Comprobar que funciona y eliminar equipo si no tiene jugadores</t>
+    <t>Eliminar organization si no tiene equipo</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>31</v>
@@ -637,7 +637,9 @@
       <c r="B10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
BE delete team without player and being an administrator
</commit_message>
<xml_diff>
--- a/Tasks/Views.xlsx
+++ b/Tasks/Views.xlsx
@@ -118,10 +118,10 @@
     <t>Seria necesario un mejor control de errores.</t>
   </si>
   <si>
-    <t>Eliminar organization (grupo) si no tiene equipos</t>
-  </si>
-  <si>
     <t>Eliminar organization si no tiene equipo</t>
+  </si>
+  <si>
+    <t>Comprobar eliminar organization</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,10 +635,10 @@
         <v>12</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D10" s="4"/>
     </row>

</xml_diff>

<commit_message>
back de crear partido no necesario
</commit_message>
<xml_diff>
--- a/Tasks/Views.xlsx
+++ b/Tasks/Views.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>MockUp</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Seria necesario un mejor control de errores.</t>
+  </si>
+  <si>
+    <t>No es necesario</t>
   </si>
 </sst>
 </file>
@@ -509,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +574,9 @@
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
     </row>

</xml_diff>

<commit_message>
esqueleto para crear partido
</commit_message>
<xml_diff>
--- a/Tasks/Views.xlsx
+++ b/Tasks/Views.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>MockUp</t>
   </si>
@@ -112,7 +112,13 @@
     <t>Seria necesario un mejor control de errores.</t>
   </si>
   <si>
-    <t>No es necesario</t>
+    <t>Por ahora no se realizará, se hará directamente seleccionar equipos</t>
+  </si>
+  <si>
+    <t>Se llamará Create  Match en la parte front y estará fusionada con configuracion equipo</t>
+  </si>
+  <si>
+    <t>Se llamara Create Team, solo corresponderá a la parte de seleccionar equipos</t>
   </si>
 </sst>
 </file>
@@ -513,7 +519,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +527,7 @@
     <col min="1" max="1" width="37.140625" customWidth="1"/>
     <col min="2" max="2" width="59.28515625" customWidth="1"/>
     <col min="3" max="3" width="59.85546875" customWidth="1"/>
-    <col min="4" max="4" width="60" customWidth="1"/>
+    <col min="4" max="4" width="78" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -544,7 +550,9 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -571,14 +579,14 @@
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -597,12 +605,14 @@
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -735,12 +745,14 @@
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">

</xml_diff>